<commit_message>
modified application report and added contects
</commit_message>
<xml_diff>
--- a/附件4：2019年大学生创新创业训练计划项目信息表.xlsx
+++ b/附件4：2019年大学生创新创业训练计划项目信息表.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e浏览器下载\Utah\省级_文华_基于 Spark 平台的人工智能知识的知识图谱构建\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4C43C5-836A-4B29-9790-F2991CCDC43B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="9456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result_190304_1641" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>2019年大学生创新创业训练计划项目信息表</t>
   </si>
@@ -62,14 +68,54 @@
   </si>
   <si>
     <t>编号</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机与信息系</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>创新</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>省级</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>文华</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机科学与技术</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>随着计算机大数据的快速发展，可以借助于互联网平台的各种工具找到有价值内容，但海量数据給筛选、组织与评价带来极大困难。 项目拟利用分布式爬虫实现PathFinder 算法获得学科信息并借助 Spark 平台过滤无效信息，再借助 Spark 优化基于词向量的文本特征选择算法完成学科专有名词分类， 同时采用 Bayes 统计推断完成关键词与相关信息的联想，完成内容的可视化。项目意义在于通过 Spark 完成人工智能知识的重整，实现了一个学习者尤其是本科生适用的知识图谱工具。</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于Spark平台的人工智能知识的知识图谱构建</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>尧铖2017217987,刘宏鑫2017217989,周余2017218005</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统需要修改</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗月童（教授）</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +310,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -446,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -576,6 +628,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -705,7 +768,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -721,6 +784,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,24 +801,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -761,24 +833,32 @@
     <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -820,7 +900,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -852,9 +932,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -886,6 +984,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1061,18 +1177,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.77734375" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
@@ -1081,103 +1198,134 @@
     <col min="14" max="14" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="12">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="12">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.399999999999999">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>520</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2017218007</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="4">
+        <v>8000</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1193,7 +1341,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1209,7 +1357,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1225,7 +1373,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1241,7 +1389,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1257,7 +1405,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1273,7 +1421,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1289,7 +1437,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1305,7 +1453,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1321,7 +1469,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1337,7 +1485,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1353,7 +1501,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1596,5 +1744,6 @@
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>